<commit_message>
changes in ddd file for changes in datatype instead of datetime change to timestamp
</commit_message>
<xml_diff>
--- a/Documents/Database Design Document.xlsx
+++ b/Documents/Database Design Document.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Scope" sheetId="3" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>EstablishedDate</t>
   </si>
   <si>
-    <t>RecordCreateDateTime</t>
-  </si>
-  <si>
     <t>DataType</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
     <t>fk_Addr_ID(EntityeAddressDetails)</t>
   </si>
   <si>
@@ -215,9 +209,6 @@
     <t>UniqueID</t>
   </si>
   <si>
-    <t>RecordModifiedDateTime</t>
-  </si>
-  <si>
     <t>BloodGroup</t>
   </si>
   <si>
@@ -548,9 +539,6 @@
     <t>Scope :</t>
   </si>
   <si>
-    <t>To identify verious tables needed for database</t>
-  </si>
-  <si>
     <t>Version :</t>
   </si>
   <si>
@@ -561,6 +549,18 @@
   </si>
   <si>
     <t>MAS and RD</t>
+  </si>
+  <si>
+    <t>To identify various tables needed for database</t>
+  </si>
+  <si>
+    <t>RecordCreateTIMESTAMP</t>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>RecordModifiedTIMESTAMP</t>
   </si>
 </sst>
 </file>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,42 +992,42 @@
   <sheetData>
     <row r="5" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E5" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E6" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E7" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E8" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E9" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="5:6" x14ac:dyDescent="0.25">
@@ -1061,24 +1061,24 @@
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G5" s="11">
         <v>1</v>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G6" s="11">
         <v>2</v>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1130,11 +1130,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G7" s="11">
         <v>3</v>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G8" s="11">
         <v>4</v>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -1174,19 +1174,19 @@
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -1194,11 +1194,11 @@
         <v>6</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1278,11 +1278,11 @@
         <v>13</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1290,16 +1290,16 @@
         <v>14</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1323,7 +1323,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -1341,9 +1341,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1362,7 @@
         <v>24</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1378,10 +1378,10 @@
         <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1389,26 +1389,26 @@
         <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1416,23 +1416,23 @@
         <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1448,21 +1448,21 @@
         <v>26</v>
       </c>
       <c r="H13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1470,26 +1470,26 @@
         <v>27</v>
       </c>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1497,34 +1497,34 @@
         <v>28</v>
       </c>
       <c r="H18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H20" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H21" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1540,123 +1540,123 @@
         <v>26</v>
       </c>
       <c r="H24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H36" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H37" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1664,7 +1664,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1672,131 +1672,131 @@
         <v>26</v>
       </c>
       <c r="H41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I41" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I42" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H43" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H45" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H46" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H47" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I50" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H52" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H53" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H54" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H55" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
         <v>5</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -1812,26 +1812,26 @@
         <v>26</v>
       </c>
       <c r="H58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H59" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H60" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>6</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -1847,109 +1847,109 @@
         <v>26</v>
       </c>
       <c r="H63" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I63" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I64" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H66" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H68" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H69" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H70" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H71" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H72" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H74" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H75" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1965,21 +1965,21 @@
         <v>26</v>
       </c>
       <c r="H78" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I78" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H79" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I79" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -1987,58 +1987,58 @@
         <v>27</v>
       </c>
       <c r="H80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H81" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I84" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H85" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H86" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2054,21 +2054,21 @@
         <v>26</v>
       </c>
       <c r="H89" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I89" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F90" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H90" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I90" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -2076,7 +2076,7 @@
         <v>27</v>
       </c>
       <c r="H91" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -2084,69 +2084,69 @@
         <v>2</v>
       </c>
       <c r="H92" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I92" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F93" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H93" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F94" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H94" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F95" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H95" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F96" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H96" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F97" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H97" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I97" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F98" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H98" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F99" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H99" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2162,34 +2162,34 @@
         <v>26</v>
       </c>
       <c r="H102" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I102" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F103" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H103" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F104" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H104" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F105" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H105" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
         <v>10</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -2205,66 +2205,66 @@
         <v>26</v>
       </c>
       <c r="H108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I108" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F109" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H109" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F110" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H110" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F111" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H111" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F112" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F113" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F114" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H114" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F115" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H115" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
         <v>11</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -2280,26 +2280,26 @@
         <v>26</v>
       </c>
       <c r="H118" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I118" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F119" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H119" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F120" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H120" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>12</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -2315,18 +2315,18 @@
         <v>26</v>
       </c>
       <c r="H123" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I123" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F124" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H124" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="127" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2342,10 +2342,10 @@
         <v>26</v>
       </c>
       <c r="H128" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I128" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -2353,10 +2353,10 @@
         <v>0</v>
       </c>
       <c r="H129" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I129" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -2364,18 +2364,18 @@
         <v>2</v>
       </c>
       <c r="H130" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I130" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F131" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H131" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -2383,72 +2383,72 @@
         <v>1</v>
       </c>
       <c r="H132" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I132" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F133" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H133" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F134" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H134" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F135" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H135" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F136" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H136" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I136" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F137" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H137" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I137" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F138" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H138" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F139" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H139" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>14</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -2464,110 +2464,110 @@
         <v>26</v>
       </c>
       <c r="H142" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I142" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F143" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H143" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F144" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H144" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F145" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H145" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I145" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F146" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H146" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F147" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H147" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I147" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F148" t="s">
+        <v>119</v>
+      </c>
+      <c r="H148" t="s">
+        <v>41</v>
+      </c>
+      <c r="I148" t="s">
         <v>122</v>
-      </c>
-      <c r="H148" t="s">
-        <v>42</v>
-      </c>
-      <c r="I148" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F149" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H149" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I149" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F150" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H150" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I150" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F151" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H151" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F152" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H152" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="154" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2583,29 +2583,29 @@
         <v>26</v>
       </c>
       <c r="H155" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I155" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F156" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H156" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I156" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F157" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H157" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -2613,21 +2613,21 @@
         <v>0</v>
       </c>
       <c r="H158" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I158" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F159" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H159" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I159" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -2635,10 +2635,10 @@
         <v>1</v>
       </c>
       <c r="H160" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I160" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -2646,53 +2646,53 @@
         <v>2</v>
       </c>
       <c r="H161" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I161" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F162" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H162" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F163" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H163" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F164" t="s">
+        <v>132</v>
+      </c>
+      <c r="H164" t="s">
+        <v>40</v>
+      </c>
+      <c r="I164" t="s">
         <v>135</v>
-      </c>
-      <c r="H164" t="s">
-        <v>41</v>
-      </c>
-      <c r="I164" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F165" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H165" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F166" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H166" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="168" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2708,29 +2708,29 @@
         <v>26</v>
       </c>
       <c r="H169" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I169" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F170" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H170" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I170" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F171" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H171" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -2738,10 +2738,10 @@
         <v>0</v>
       </c>
       <c r="H172" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I172" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -2749,61 +2749,61 @@
         <v>3</v>
       </c>
       <c r="H173" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I173" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F174" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H174" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F175" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H175" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F176" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H176" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="177" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F177" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H177" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I177" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="178" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F178" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H178" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="179" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F179" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H179" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2820,7 @@
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2839,7 +2839,7 @@
         <v>24</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2856,39 +2856,39 @@
         <v>26</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2904,23 +2904,23 @@
         <v>26</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H12" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2928,7 +2928,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2936,45 +2936,45 @@
         <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="H18" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="H19" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in ddd file - instead of Bit change to number(1) as datatype
</commit_message>
<xml_diff>
--- a/Documents/Database Design Document.xlsx
+++ b/Documents/Database Design Document.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Scope" sheetId="3" r:id="rId1"/>
@@ -269,9 +269,6 @@
     <t>Level</t>
   </si>
   <si>
-    <t>Fess</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -416,9 +413,6 @@
     <t>IsAbsent</t>
   </si>
   <si>
-    <t>Bit</t>
-  </si>
-  <si>
     <t>FacultyAttendance</t>
   </si>
   <si>
@@ -561,6 +555,12 @@
   </si>
   <si>
     <t>RecordModifiedTIMESTAMP</t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>NUMBER(1)</t>
   </si>
 </sst>
 </file>
@@ -992,42 +992,42 @@
   <sheetData>
     <row r="5" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E5" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E6" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E7" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E8" s="16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="5:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E9" s="16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="5:6" x14ac:dyDescent="0.25">
@@ -1061,24 +1061,24 @@
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G5" s="11">
         <v>1</v>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G6" s="11">
         <v>2</v>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1130,11 +1130,11 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G7" s="11">
         <v>3</v>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G8" s="11">
         <v>4</v>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="14" t="s">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -1198,7 +1198,7 @@
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -1278,11 +1278,11 @@
         <v>13</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1294,12 +1294,12 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1323,7 +1323,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -1341,9 +1341,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F169" sqref="F169:H179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,7 +1381,7 @@
         <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1421,18 +1421,18 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1451,7 +1451,7 @@
         <v>41</v>
       </c>
       <c r="I13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>40</v>
       </c>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1513,18 +1513,18 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1543,7 +1543,7 @@
         <v>41</v>
       </c>
       <c r="I24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
         <v>40</v>
       </c>
       <c r="I25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1645,18 +1645,18 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
         <v>41</v>
       </c>
       <c r="I41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>40</v>
       </c>
       <c r="I42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1785,18 +1785,18 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H54" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H55" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1815,7 +1815,7 @@
         <v>41</v>
       </c>
       <c r="I58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -1828,10 +1828,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H60" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1850,7 +1850,7 @@
         <v>40</v>
       </c>
       <c r="I63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>41</v>
       </c>
       <c r="I64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -1938,18 +1938,18 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H74" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H75" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1968,7 +1968,7 @@
         <v>41</v>
       </c>
       <c r="I78" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -1979,7 +1979,7 @@
         <v>40</v>
       </c>
       <c r="I79" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -2000,7 +2000,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H82" t="s">
         <v>41</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
-        <v>80</v>
+        <v>176</v>
       </c>
       <c r="H83" t="s">
         <v>41</v>
@@ -2027,18 +2027,18 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H85" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H86" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2057,7 +2057,7 @@
         <v>41</v>
       </c>
       <c r="I89" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
         <v>40</v>
       </c>
       <c r="I90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F93" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H93" t="s">
         <v>58</v>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F94" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H94" t="s">
         <v>41</v>
@@ -2135,18 +2135,18 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F98" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H98" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F99" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H99" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2165,12 +2165,12 @@
         <v>40</v>
       </c>
       <c r="I102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F103" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H103" t="s">
         <v>50</v>
@@ -2178,18 +2178,18 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F104" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H104" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F105" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H105" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
         <v>10</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -2208,12 +2208,12 @@
         <v>40</v>
       </c>
       <c r="I108" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F109" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H109" t="s">
         <v>50</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F110" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H110" t="s">
         <v>50</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F111" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H111" t="s">
         <v>51</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F113" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H113" t="s">
         <v>38</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F114" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H114" t="s">
         <v>38</v>
@@ -2261,10 +2261,10 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F115" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H115" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
         <v>11</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>41</v>
       </c>
       <c r="I118" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -2291,15 +2291,15 @@
         <v>62</v>
       </c>
       <c r="H119" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F120" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H120" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="122" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
         <v>12</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -2318,15 +2318,15 @@
         <v>41</v>
       </c>
       <c r="I123" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F124" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H124" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="127" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>40</v>
       </c>
       <c r="I128" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -2356,7 +2356,7 @@
         <v>40</v>
       </c>
       <c r="I129" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -2367,12 +2367,12 @@
         <v>40</v>
       </c>
       <c r="I130" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F131" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H131" t="s">
         <v>40</v>
@@ -2386,12 +2386,12 @@
         <v>40</v>
       </c>
       <c r="I132" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F133" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H133" t="s">
         <v>41</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F134" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H134" t="s">
         <v>41</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F135" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H135" t="s">
         <v>41</v>
@@ -2415,40 +2415,40 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F136" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H136" t="s">
         <v>40</v>
       </c>
       <c r="I136" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F137" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H137" t="s">
         <v>41</v>
       </c>
       <c r="I137" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F138" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H138" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F139" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H139" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
         <v>14</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -2467,12 +2467,12 @@
         <v>40</v>
       </c>
       <c r="I142" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F143" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H143" t="s">
         <v>50</v>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F144" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H144" t="s">
         <v>50</v>
@@ -2488,13 +2488,13 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F145" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H145" t="s">
         <v>51</v>
       </c>
       <c r="I145" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -2513,61 +2513,61 @@
         <v>40</v>
       </c>
       <c r="I147" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F148" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H148" t="s">
         <v>41</v>
       </c>
       <c r="I148" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F149" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H149" t="s">
         <v>41</v>
       </c>
       <c r="I149" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F150" t="s">
+        <v>119</v>
+      </c>
+      <c r="H150" t="s">
+        <v>40</v>
+      </c>
+      <c r="I150" t="s">
         <v>120</v>
-      </c>
-      <c r="H150" t="s">
-        <v>40</v>
-      </c>
-      <c r="I150" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F151" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H151" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F152" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H152" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="154" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2586,7 +2586,7 @@
         <v>41</v>
       </c>
       <c r="I155" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -2597,7 +2597,7 @@
         <v>40</v>
       </c>
       <c r="I156" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -2616,18 +2616,18 @@
         <v>40</v>
       </c>
       <c r="I158" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F159" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H159" t="s">
         <v>40</v>
       </c>
       <c r="I159" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>40</v>
       </c>
       <c r="I160" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -2649,50 +2649,50 @@
         <v>40</v>
       </c>
       <c r="I161" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F162" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H162" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F163" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H163" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F164" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H164" t="s">
         <v>40</v>
       </c>
       <c r="I164" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F165" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H165" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F166" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H166" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="168" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2711,7 +2711,7 @@
         <v>41</v>
       </c>
       <c r="I169" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -2722,15 +2722,15 @@
         <v>40</v>
       </c>
       <c r="I170" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F171" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H171" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -2741,7 +2741,7 @@
         <v>40</v>
       </c>
       <c r="I172" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -2752,58 +2752,58 @@
         <v>41</v>
       </c>
       <c r="I173" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F174" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H174" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F175" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H175" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F176" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H176" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="177" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F177" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H177" t="s">
         <v>40</v>
       </c>
       <c r="I177" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="178" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F178" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H178" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="179" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F179" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H179" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2816,11 +2816,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2847,7 +2847,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2861,7 +2861,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
         <v>38</v>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
         <v>58</v>
@@ -2877,18 +2877,18 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2909,18 +2909,18 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" t="s">
         <v>88</v>
-      </c>
-      <c r="H11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2928,7 +2928,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2941,40 +2941,40 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H16" t="s">
         <v>40</v>
       </c>
       <c r="I16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" t="s">
         <v>40</v>
       </c>
       <c r="I17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some changes made on DDD file
</commit_message>
<xml_diff>
--- a/Documents/Database Design Document.xlsx
+++ b/Documents/Database Design Document.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Scope" sheetId="3" r:id="rId1"/>
@@ -1341,9 +1341,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F169" sqref="F169:H179"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2816,7 +2816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>